<commit_message>
ultima version del proyecto
</commit_message>
<xml_diff>
--- a/public/file_user_excel/Formato_de_Solicitud_de_Materiales_y_Servicios.xlsx
+++ b/public/file_user_excel/Formato_de_Solicitud_de_Materiales_y_Servicios.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costos01\Dropbox\ESTRUCTURA DE COSTOS\Analisis de Costos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7755"/>
   </bookViews>
@@ -19,12 +14,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilla de solicitud de Serv.'!$C$7:$O$94</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Planilla de solicitud de Mat.'!$A$1:$G$56</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="170">
   <si>
     <t>Lista de Corte</t>
   </si>
@@ -549,18 +544,21 @@
   <si>
     <t>Nº Ppto:</t>
   </si>
+  <si>
+    <t>Modificado 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;Bs.S&quot;* #,##0.00_ ;_ &quot;Bs.S&quot;* \-#,##0.00_ ;_ &quot;Bs.S&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0_ ;\-0\ "/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;Bs.S&quot;* #,##0.00_ ;_ &quot;Bs.S&quot;* \-#,##0.00_ ;_ &quot;Bs.S&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="46">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1519,7 +1517,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1549,27 +1547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1609,10 +1586,10 @@
     <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="45" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
@@ -1738,7 +1715,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="43" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="43" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="35" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1787,6 +1764,27 @@
     </xf>
     <xf numFmtId="49" fontId="45" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1808,11 +1806,10 @@
     <cellStyle name="60% - Énfasis4" xfId="32" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="36" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="40" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="21" builtinId="33" customBuiltin="1"/>
@@ -1834,6 +1831,7 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="15" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -1871,7 +1869,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D40D79F2-8C2F-485F-8847-76E9C2807754}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D40D79F2-8C2F-485F-8847-76E9C2807754}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1883,7 +1881,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1952,7 +1950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1984,10 +1982,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2019,7 +2016,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2195,712 +2191,717 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="80" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="80" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" style="81" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="80" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="80" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="79" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="79" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="79"/>
+    <col min="1" max="1" width="6.85546875" style="73" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="73" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" style="74" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="73" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="73" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="72" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="72" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="131" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="142"/>
-      <c r="B1" s="136"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-    </row>
-    <row r="2" spans="1:7" s="131" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="137" t="s">
+    <row r="1" spans="1:7" s="124" customFormat="1" ht="79.5" customHeight="1">
+      <c r="A1" s="135"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+    </row>
+    <row r="2" spans="1:7" s="124" customFormat="1" ht="15.75">
+      <c r="A2" s="130" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="136"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="139" t="s">
+      <c r="B2" s="129"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="132" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="155" t="s">
+      <c r="E2" s="148" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="131" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+    <row r="3" spans="1:7" s="124" customFormat="1" ht="15.75">
+      <c r="A3" s="130" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="139" t="s">
+      <c r="B3" s="129"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="132" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="138"/>
-    </row>
-    <row r="4" spans="1:7" s="131" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="137" t="s">
+      <c r="E3" s="131"/>
+    </row>
+    <row r="4" spans="1:7" s="124" customFormat="1" ht="12.75">
+      <c r="A4" s="130" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="136"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-    </row>
-    <row r="5" spans="1:7" s="131" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="137" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+    </row>
+    <row r="5" spans="1:7" s="124" customFormat="1" ht="12.75">
+      <c r="A5" s="130" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
-    </row>
-    <row r="6" spans="1:7" s="131" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="136"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-    </row>
-    <row r="7" spans="1:7" s="112" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="117"/>
-      <c r="B7" s="116" t="s">
+      <c r="B5" s="129"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+    </row>
+    <row r="6" spans="1:7" s="124" customFormat="1" ht="6" customHeight="1">
+      <c r="A6" s="129"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+    </row>
+    <row r="7" spans="1:7" s="105" customFormat="1">
+      <c r="A7" s="110"/>
+      <c r="B7" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="114"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-    </row>
-    <row r="8" spans="1:7" s="112" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="117"/>
-      <c r="B8" s="116" t="s">
+      <c r="D7" s="107"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+    </row>
+    <row r="8" spans="1:7" s="105" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A8" s="110"/>
+      <c r="B8" s="109" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="151"/>
-      <c r="G8" s="151"/>
-    </row>
-    <row r="9" spans="1:7" s="128" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="130"/>
-      <c r="B9" s="116" t="s">
+      <c r="C8" s="108"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="144"/>
+    </row>
+    <row r="9" spans="1:7" s="121" customFormat="1">
+      <c r="A9" s="123"/>
+      <c r="B9" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="108" t="s">
         <v>165</v>
       </c>
-      <c r="D9" s="130"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="152"/>
-      <c r="G9" s="152"/>
-    </row>
-    <row r="10" spans="1:7" s="112" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="117"/>
-      <c r="B10" s="116" t="s">
+      <c r="D9" s="123"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="145"/>
+    </row>
+    <row r="10" spans="1:7" s="105" customFormat="1">
+      <c r="A10" s="110"/>
+      <c r="B10" s="109" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="115"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-    </row>
-    <row r="11" spans="1:7" s="112" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="117"/>
-      <c r="B11" s="116" t="s">
+      <c r="C10" s="108"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+    </row>
+    <row r="11" spans="1:7" s="105" customFormat="1">
+      <c r="A11" s="110"/>
+      <c r="B11" s="109" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="115"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="127"/>
-    </row>
-    <row r="12" spans="1:7" s="120" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="126"/>
-      <c r="B12" s="125" t="s">
+      <c r="C11" s="108"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+    </row>
+    <row r="12" spans="1:7" s="113" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A12" s="119"/>
+      <c r="B12" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="108" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-    </row>
-    <row r="13" spans="1:7" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="126"/>
-      <c r="B13" s="125" t="s">
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+    </row>
+    <row r="13" spans="1:7" s="113" customFormat="1">
+      <c r="A13" s="119"/>
+      <c r="B13" s="118" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="124"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="122"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-    </row>
-    <row r="14" spans="1:7" s="112" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
-      <c r="B14" s="116" t="s">
+      <c r="C13" s="117"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+    </row>
+    <row r="14" spans="1:7" s="105" customFormat="1">
+      <c r="A14" s="110"/>
+      <c r="B14" s="109" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-    </row>
-    <row r="15" spans="1:7" s="112" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="117"/>
-      <c r="B15" s="116" t="s">
+      <c r="C14" s="108"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+    </row>
+    <row r="15" spans="1:7" s="105" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A15" s="110"/>
+      <c r="B15" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-    </row>
-    <row r="16" spans="1:7" s="112" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117"/>
-      <c r="B16" s="116" t="s">
+      <c r="C15" s="108"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+    </row>
+    <row r="16" spans="1:7" s="105" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A16" s="110"/>
+      <c r="B16" s="109" t="s">
         <v>136</v>
       </c>
-      <c r="C16" s="115"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="113"/>
-    </row>
-    <row r="17" spans="1:8" s="110" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="111" t="s">
+      <c r="C16" s="108"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="106"/>
+    </row>
+    <row r="17" spans="1:8" s="103" customFormat="1">
+      <c r="A17" s="104" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="111" t="s">
+      <c r="B17" s="104" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="109" t="s">
+      <c r="D17" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="109" t="s">
+      <c r="E17" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="111" t="s">
+      <c r="F17" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="G17" s="111" t="s">
+      <c r="G17" s="104" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="106"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="144"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-    </row>
-    <row r="19" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="106"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="153" t="s">
+    <row r="18" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="99"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+    </row>
+    <row r="19" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="99"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="146" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
-    </row>
-    <row r="20" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="106">
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+    </row>
+    <row r="20" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A20" s="99">
         <v>1</v>
       </c>
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="154" t="s">
+      <c r="C20" s="147" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="147">
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="140">
         <v>2</v>
       </c>
-      <c r="G20" s="147" t="s">
+      <c r="G20" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="149"/>
-    </row>
-    <row r="21" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="106">
+      <c r="H20" s="142"/>
+    </row>
+    <row r="21" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A21" s="99">
         <v>2</v>
       </c>
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="154" t="s">
+      <c r="C21" s="147" t="s">
         <v>152</v>
       </c>
-      <c r="D21" s="146"/>
-      <c r="E21" s="146"/>
-      <c r="F21" s="147">
+      <c r="D21" s="139"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="140">
         <v>3</v>
       </c>
-      <c r="G21" s="147" t="s">
+      <c r="G21" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="H21" s="149"/>
-    </row>
-    <row r="22" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="106">
+      <c r="H21" s="142"/>
+    </row>
+    <row r="22" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A22" s="99">
         <v>3</v>
       </c>
-      <c r="B22" s="143" t="s">
+      <c r="B22" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="154" t="s">
+      <c r="C22" s="147" t="s">
         <v>153</v>
       </c>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="147">
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="140">
         <v>5</v>
       </c>
-      <c r="G22" s="147" t="s">
+      <c r="G22" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="149"/>
-    </row>
-    <row r="23" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="146"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="149"/>
-    </row>
-    <row r="24" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="106"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="153" t="s">
+      <c r="H22" s="142"/>
+    </row>
+    <row r="23" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="99"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
+      <c r="H23" s="142"/>
+    </row>
+    <row r="24" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A24" s="99"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="146" t="s">
         <v>157</v>
       </c>
-      <c r="D24" s="145"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="145"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="149"/>
-    </row>
-    <row r="25" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="106">
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="142"/>
+    </row>
+    <row r="25" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="99">
         <v>4</v>
       </c>
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="154" t="s">
+      <c r="C25" s="147" t="s">
         <v>155</v>
       </c>
-      <c r="D25" s="145"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145">
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138">
         <v>10</v>
       </c>
-      <c r="G25" s="145" t="s">
+      <c r="G25" s="138" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="106">
+    <row r="26" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A26" s="99">
         <v>5</v>
       </c>
-      <c r="B26" s="143" t="s">
+      <c r="B26" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="154" t="s">
+      <c r="C26" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="145">
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138">
         <v>5</v>
       </c>
-      <c r="G26" s="145" t="s">
+      <c r="G26" s="138" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
-      <c r="B27" s="143"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
-    </row>
-    <row r="28" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="106"/>
-      <c r="B28" s="143"/>
-      <c r="C28" s="153" t="s">
+    <row r="27" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A27" s="99"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
+    </row>
+    <row r="28" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A28" s="99"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="146" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="149"/>
-    </row>
-    <row r="29" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106">
+      <c r="D28" s="138"/>
+      <c r="E28" s="138"/>
+      <c r="F28" s="138"/>
+      <c r="G28" s="138"/>
+      <c r="H28" s="142"/>
+    </row>
+    <row r="29" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A29" s="99">
         <v>6</v>
       </c>
-      <c r="B29" s="143" t="s">
+      <c r="B29" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C29" s="154" t="s">
+      <c r="C29" s="147" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="145"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="145">
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="138">
         <v>5</v>
       </c>
-      <c r="G29" s="145" t="s">
+      <c r="G29" s="138" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="106">
+    <row r="30" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="99">
         <v>7</v>
       </c>
-      <c r="B30" s="143" t="s">
+      <c r="B30" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="154" t="s">
+      <c r="C30" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="145">
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="138">
         <v>4</v>
       </c>
-      <c r="G30" s="145" t="s">
+      <c r="G30" s="138" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="106"/>
-      <c r="B31" s="143"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="145"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="145"/>
-      <c r="G31" s="145"/>
-    </row>
-    <row r="32" spans="1:8" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="106"/>
-      <c r="B32" s="143"/>
-      <c r="C32" s="153" t="s">
+    <row r="31" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="99"/>
+      <c r="B31" s="136"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
+    </row>
+    <row r="32" spans="1:8" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="99"/>
+      <c r="B32" s="136"/>
+      <c r="C32" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="145"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="145"/>
-      <c r="G32" s="145"/>
-    </row>
-    <row r="33" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="106">
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="138"/>
+    </row>
+    <row r="33" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="99">
         <v>8</v>
       </c>
-      <c r="B33" s="143" t="s">
+      <c r="B33" s="136" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="154" t="s">
+      <c r="C33" s="147" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="145"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="145">
+      <c r="D33" s="138"/>
+      <c r="E33" s="138"/>
+      <c r="F33" s="138">
         <v>3</v>
       </c>
-      <c r="G33" s="145" t="s">
+      <c r="G33" s="138" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="106"/>
-      <c r="B34" s="143"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="145"/>
-      <c r="E34" s="145"/>
-      <c r="F34" s="145"/>
-      <c r="G34" s="145"/>
-    </row>
-    <row r="35" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
-      <c r="B35" s="143"/>
-      <c r="C35" s="153" t="s">
+    <row r="34" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="99"/>
+      <c r="B34" s="136"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="138"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="138"/>
+    </row>
+    <row r="35" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="99"/>
+      <c r="B35" s="136"/>
+      <c r="C35" s="146" t="s">
         <v>163</v>
       </c>
-      <c r="D35" s="145"/>
-      <c r="E35" s="145"/>
-      <c r="F35" s="145"/>
-      <c r="G35" s="145"/>
-    </row>
-    <row r="36" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="106"/>
-      <c r="B36" s="143"/>
-      <c r="C36" s="154" t="s">
+      <c r="D35" s="138"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="138"/>
+    </row>
+    <row r="36" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="99"/>
+      <c r="B36" s="136"/>
+      <c r="C36" s="147" t="s">
         <v>151</v>
       </c>
-      <c r="D36" s="145"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="145">
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138">
         <v>50</v>
       </c>
-      <c r="G36" s="145" t="s">
+      <c r="G36" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="106"/>
-      <c r="B37" s="143"/>
-      <c r="C37" s="154" t="s">
+    <row r="37" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="99"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="147" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="145"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="145">
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138">
         <v>75</v>
       </c>
-      <c r="G37" s="145" t="s">
+      <c r="G37" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="106"/>
-      <c r="B38" s="143"/>
-      <c r="C38" s="154" t="s">
+    <row r="38" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="99"/>
+      <c r="B38" s="136"/>
+      <c r="C38" s="147" t="s">
         <v>153</v>
       </c>
-      <c r="D38" s="145"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="145">
+      <c r="D38" s="138"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138">
         <v>125</v>
       </c>
-      <c r="G38" s="145" t="s">
+      <c r="G38" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="106"/>
-      <c r="B39" s="143"/>
-      <c r="C39" s="144"/>
-      <c r="D39" s="145"/>
-      <c r="E39" s="145"/>
-      <c r="F39" s="145"/>
-      <c r="G39" s="145"/>
-    </row>
-    <row r="40" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106"/>
-      <c r="B40" s="143"/>
-      <c r="C40" s="153" t="s">
+    <row r="39" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="99"/>
+      <c r="B39" s="136"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="138"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="138"/>
+    </row>
+    <row r="40" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A40" s="99"/>
+      <c r="B40" s="136"/>
+      <c r="C40" s="146" t="s">
         <v>164</v>
       </c>
-      <c r="D40" s="145"/>
-      <c r="E40" s="145"/>
-      <c r="F40" s="145"/>
-      <c r="G40" s="145"/>
-    </row>
-    <row r="41" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="106"/>
-      <c r="B41" s="143"/>
-      <c r="C41" s="154" t="s">
+      <c r="D40" s="138"/>
+      <c r="E40" s="138"/>
+      <c r="F40" s="138"/>
+      <c r="G40" s="138"/>
+    </row>
+    <row r="41" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="99"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="147" t="s">
         <v>155</v>
       </c>
-      <c r="D41" s="145"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="145">
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138">
         <v>250</v>
       </c>
-      <c r="G41" s="145" t="s">
+      <c r="G41" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="106"/>
-      <c r="B42" s="143"/>
-      <c r="C42" s="154" t="s">
+    <row r="42" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="99"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D42" s="145"/>
-      <c r="E42" s="145"/>
-      <c r="F42" s="145">
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138">
         <v>125</v>
       </c>
-      <c r="G42" s="145" t="s">
+      <c r="G42" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="106"/>
-      <c r="B43" s="143"/>
-      <c r="C43" s="154" t="s">
+    <row r="43" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="99"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="147" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="145"/>
-      <c r="E43" s="145"/>
-      <c r="F43" s="145">
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="F43" s="138">
         <v>125</v>
       </c>
-      <c r="G43" s="145" t="s">
+      <c r="G43" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="97" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="106"/>
-      <c r="B44" s="143"/>
-      <c r="C44" s="154" t="s">
+    <row r="44" spans="1:7" s="90" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A44" s="99"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="145"/>
-      <c r="E44" s="145"/>
-      <c r="F44" s="145">
+      <c r="D44" s="138"/>
+      <c r="E44" s="138"/>
+      <c r="F44" s="138">
         <v>100</v>
       </c>
-      <c r="G44" s="145" t="s">
+      <c r="G44" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="97" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="106"/>
-      <c r="B45" s="143"/>
-      <c r="C45" s="104"/>
-      <c r="D45" s="146"/>
-      <c r="E45" s="146"/>
-      <c r="F45" s="148"/>
-      <c r="G45" s="148"/>
-    </row>
-    <row r="46" spans="1:7" s="97" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="106"/>
-      <c r="B46" s="105"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="103"/>
-      <c r="E46" s="103"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="103"/>
-    </row>
-    <row r="47" spans="1:7" s="97" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="84"/>
-      <c r="B47" s="102"/>
-      <c r="C47" s="101"/>
-      <c r="D47" s="100"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="98"/>
-    </row>
-    <row r="48" spans="1:7" s="83" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="84"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="84"/>
-    </row>
-    <row r="49" spans="1:7" s="83" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="94" t="s">
+    <row r="45" spans="1:7" s="90" customFormat="1" ht="15">
+      <c r="A45" s="99"/>
+      <c r="B45" s="136"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="141"/>
+      <c r="G45" s="141"/>
+    </row>
+    <row r="46" spans="1:7" s="90" customFormat="1" ht="15">
+      <c r="A46" s="99"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+    </row>
+    <row r="47" spans="1:7" s="90" customFormat="1">
+      <c r="A47" s="77"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="92"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="91"/>
+    </row>
+    <row r="48" spans="1:7" s="76" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="77"/>
+      <c r="B48" s="89"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="77"/>
+    </row>
+    <row r="49" spans="1:7" s="76" customFormat="1" ht="15" customHeight="1">
+      <c r="A49" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="86"/>
-    </row>
-    <row r="50" spans="1:7" s="83" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="85" t="s">
+      <c r="B49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="79"/>
+    </row>
+    <row r="50" spans="1:7" s="76" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A50" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="84"/>
-    </row>
-    <row r="51" spans="1:7" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="93">
+      <c r="B50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="77"/>
+    </row>
+    <row r="51" spans="1:7" s="76" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A51" s="86">
         <v>3</v>
       </c>
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="143" t="s">
         <v>149</v>
       </c>
-      <c r="F51" s="89"/>
-    </row>
-    <row r="52" spans="1:7" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="92" t="s">
+      <c r="F51" s="82"/>
+    </row>
+    <row r="52" spans="1:7" s="76" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B52" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="F52" s="89"/>
-    </row>
-    <row r="53" spans="1:7" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="85" t="s">
+      <c r="F52" s="82"/>
+    </row>
+    <row r="53" spans="1:7" s="76" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B53" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="89"/>
-    </row>
-    <row r="54" spans="1:7" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="91" t="s">
+      <c r="F53" s="82"/>
+    </row>
+    <row r="54" spans="1:7" s="76" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B54" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="82"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="82"/>
-      <c r="F54" s="89"/>
-    </row>
-    <row r="55" spans="1:7" s="83" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="90" t="s">
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="82"/>
+    </row>
+    <row r="55" spans="1:7" s="76" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A55" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="B55" s="82"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
-      <c r="E55" s="82"/>
-      <c r="F55" s="89"/>
-    </row>
-    <row r="56" spans="1:7" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="82" t="s">
+      <c r="B55" s="75"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="82"/>
+    </row>
+    <row r="56" spans="1:7" s="76" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A56" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="88"/>
-      <c r="F56" s="87"/>
-      <c r="G56" s="87"/>
+      <c r="B56" s="81"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="C58" s="74" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2911,7 +2912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2921,7 +2922,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
@@ -2940,7 +2941,7 @@
     <col min="17" max="17" width="24.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" ht="26.25">
       <c r="C2" s="54" t="s">
         <v>11</v>
       </c>
@@ -2949,7 +2950,7 @@
       </c>
       <c r="I2" s="54"/>
     </row>
-    <row r="3" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="20.25">
       <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
@@ -2957,21 +2958,21 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="20.25">
       <c r="C4" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="71" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="20.25">
       <c r="C5" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="78"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="71"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75">
       <c r="A6" s="57"/>
       <c r="B6" s="58"/>
       <c r="C6" s="60"/>
@@ -2983,18 +2984,18 @@
       <c r="G6" s="58"/>
       <c r="H6" s="58"/>
       <c r="I6" s="62"/>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="153" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="77"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K6" s="154"/>
+      <c r="L6" s="154"/>
+      <c r="M6" s="154"/>
+      <c r="N6" s="154"/>
+      <c r="O6" s="154"/>
+      <c r="P6" s="154"/>
+      <c r="Q6" s="155"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="61" t="s">
         <v>13</v>
       </c>
@@ -3047,7 +3048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="4" customFormat="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="48" t="s">
@@ -3068,7 +3069,7 @@
       <c r="P8" s="33"/>
       <c r="Q8" s="33"/>
     </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="16">
         <v>1</v>
       </c>
@@ -3114,7 +3115,7 @@
       <c r="Q9" s="34"/>
       <c r="S9" s="15"/>
     </row>
-    <row r="10" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" s="29" customFormat="1">
       <c r="A10" s="27">
         <v>2</v>
       </c>
@@ -3159,7 +3160,7 @@
       </c>
       <c r="Q10" s="34"/>
     </row>
-    <row r="11" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="29" customFormat="1">
       <c r="A11" s="16">
         <v>3</v>
       </c>
@@ -3204,7 +3205,7 @@
       </c>
       <c r="Q11" s="34"/>
     </row>
-    <row r="12" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" s="29" customFormat="1">
       <c r="A12" s="27">
         <v>4</v>
       </c>
@@ -3249,7 +3250,7 @@
       </c>
       <c r="Q12" s="34"/>
     </row>
-    <row r="13" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="29" customFormat="1">
       <c r="A13" s="16">
         <v>5</v>
       </c>
@@ -3294,7 +3295,7 @@
       </c>
       <c r="Q13" s="34"/>
     </row>
-    <row r="14" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="29" customFormat="1">
       <c r="A14" s="27">
         <v>6</v>
       </c>
@@ -3339,7 +3340,7 @@
       </c>
       <c r="Q14" s="34"/>
     </row>
-    <row r="15" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="29" customFormat="1">
       <c r="A15" s="16">
         <v>7</v>
       </c>
@@ -3384,7 +3385,7 @@
       </c>
       <c r="Q15" s="34"/>
     </row>
-    <row r="16" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="29" customFormat="1">
       <c r="A16" s="27">
         <v>8</v>
       </c>
@@ -3429,7 +3430,7 @@
       </c>
       <c r="Q16" s="34"/>
     </row>
-    <row r="17" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" s="29" customFormat="1">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="66" t="s">
@@ -3472,7 +3473,7 @@
       </c>
       <c r="Q17" s="55"/>
     </row>
-    <row r="18" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" s="29" customFormat="1">
       <c r="A18" s="27"/>
       <c r="B18" s="27"/>
       <c r="C18" s="59" t="s">
@@ -3493,7 +3494,7 @@
       <c r="P18" s="27"/>
       <c r="Q18" s="34"/>
     </row>
-    <row r="19" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" s="29" customFormat="1">
       <c r="A19" s="27">
         <v>9</v>
       </c>
@@ -3536,7 +3537,7 @@
       </c>
       <c r="Q19" s="34"/>
     </row>
-    <row r="20" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" s="29" customFormat="1">
       <c r="A20" s="27">
         <v>10</v>
       </c>
@@ -3579,7 +3580,7 @@
       </c>
       <c r="Q20" s="34"/>
     </row>
-    <row r="21" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" s="29" customFormat="1">
       <c r="A21" s="27">
         <v>11</v>
       </c>
@@ -3622,7 +3623,7 @@
       </c>
       <c r="Q21" s="34"/>
     </row>
-    <row r="22" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="29" customFormat="1">
       <c r="A22" s="27">
         <v>12</v>
       </c>
@@ -3665,7 +3666,7 @@
       </c>
       <c r="Q22" s="34"/>
     </row>
-    <row r="23" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="29" customFormat="1">
       <c r="A23" s="27">
         <v>13</v>
       </c>
@@ -3708,7 +3709,7 @@
       </c>
       <c r="Q23" s="34"/>
     </row>
-    <row r="24" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="29" customFormat="1">
       <c r="A24" s="27">
         <v>14</v>
       </c>
@@ -3751,7 +3752,7 @@
       </c>
       <c r="Q24" s="34"/>
     </row>
-    <row r="25" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="29" customFormat="1">
       <c r="A25" s="27">
         <v>15</v>
       </c>
@@ -3794,7 +3795,7 @@
       </c>
       <c r="Q25" s="34"/>
     </row>
-    <row r="26" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="29" customFormat="1">
       <c r="A26" s="27">
         <v>16</v>
       </c>
@@ -3837,7 +3838,7 @@
       </c>
       <c r="Q26" s="34"/>
     </row>
-    <row r="27" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="29" customFormat="1">
       <c r="A27" s="27">
         <v>17</v>
       </c>
@@ -3880,7 +3881,7 @@
       </c>
       <c r="Q27" s="34"/>
     </row>
-    <row r="28" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="29" customFormat="1">
       <c r="A28" s="27">
         <v>18</v>
       </c>
@@ -3923,7 +3924,7 @@
       </c>
       <c r="Q28" s="34"/>
     </row>
-    <row r="29" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="29" customFormat="1">
       <c r="A29" s="27">
         <v>19</v>
       </c>
@@ -3966,7 +3967,7 @@
       </c>
       <c r="Q29" s="34"/>
     </row>
-    <row r="30" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="29" customFormat="1">
       <c r="A30" s="27">
         <v>20</v>
       </c>
@@ -4009,7 +4010,7 @@
       </c>
       <c r="Q30" s="34"/>
     </row>
-    <row r="31" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="29" customFormat="1">
       <c r="A31" s="27">
         <v>21</v>
       </c>
@@ -4052,7 +4053,7 @@
       </c>
       <c r="Q31" s="34"/>
     </row>
-    <row r="32" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="29" customFormat="1">
       <c r="A32" s="27">
         <v>22</v>
       </c>
@@ -4095,7 +4096,7 @@
       </c>
       <c r="Q32" s="34"/>
     </row>
-    <row r="33" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" s="29" customFormat="1">
       <c r="A33" s="27">
         <v>23</v>
       </c>
@@ -4138,7 +4139,7 @@
       </c>
       <c r="Q33" s="34"/>
     </row>
-    <row r="34" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" s="29" customFormat="1">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
       <c r="C34" s="30"/>
@@ -4157,7 +4158,7 @@
       <c r="P34" s="27"/>
       <c r="Q34" s="34"/>
     </row>
-    <row r="35" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" s="29" customFormat="1">
       <c r="A35" s="27">
         <v>24</v>
       </c>
@@ -4200,7 +4201,7 @@
       </c>
       <c r="Q35" s="34"/>
     </row>
-    <row r="36" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="29" customFormat="1">
       <c r="A36" s="27">
         <v>25</v>
       </c>
@@ -4243,7 +4244,7 @@
       </c>
       <c r="Q36" s="34"/>
     </row>
-    <row r="37" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="29" customFormat="1">
       <c r="A37" s="27">
         <v>26</v>
       </c>
@@ -4286,7 +4287,7 @@
       </c>
       <c r="Q37" s="34"/>
     </row>
-    <row r="38" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="29" customFormat="1">
       <c r="A38" s="27">
         <v>27</v>
       </c>
@@ -4329,7 +4330,7 @@
       </c>
       <c r="Q38" s="34"/>
     </row>
-    <row r="39" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="29" customFormat="1">
       <c r="A39" s="27">
         <v>28</v>
       </c>
@@ -4372,7 +4373,7 @@
       </c>
       <c r="Q39" s="34"/>
     </row>
-    <row r="40" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="29" customFormat="1">
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
       <c r="C40" s="30"/>
@@ -4391,7 +4392,7 @@
       <c r="P40" s="27"/>
       <c r="Q40" s="34"/>
     </row>
-    <row r="41" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="29" customFormat="1">
       <c r="A41" s="27">
         <v>29</v>
       </c>
@@ -4429,12 +4430,12 @@
       <c r="O41" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P41" s="71" t="s">
+      <c r="P41" s="149" t="s">
         <v>57</v>
       </c>
       <c r="Q41" s="34"/>
     </row>
-    <row r="42" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="29" customFormat="1">
       <c r="A42" s="27">
         <v>30</v>
       </c>
@@ -4472,10 +4473,10 @@
       <c r="O42" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P42" s="74"/>
+      <c r="P42" s="152"/>
       <c r="Q42" s="34"/>
     </row>
-    <row r="43" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="29" customFormat="1">
       <c r="A43" s="27">
         <v>31</v>
       </c>
@@ -4513,10 +4514,10 @@
       <c r="O43" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P43" s="74"/>
+      <c r="P43" s="152"/>
       <c r="Q43" s="34"/>
     </row>
-    <row r="44" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="29" customFormat="1">
       <c r="A44" s="27">
         <v>32</v>
       </c>
@@ -4554,10 +4555,10 @@
       <c r="O44" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P44" s="74"/>
+      <c r="P44" s="152"/>
       <c r="Q44" s="34"/>
     </row>
-    <row r="45" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" s="29" customFormat="1">
       <c r="A45" s="27">
         <v>33</v>
       </c>
@@ -4595,10 +4596,10 @@
       <c r="O45" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P45" s="74"/>
+      <c r="P45" s="152"/>
       <c r="Q45" s="34"/>
     </row>
-    <row r="46" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" s="29" customFormat="1">
       <c r="A46" s="27">
         <v>34</v>
       </c>
@@ -4636,10 +4637,10 @@
       <c r="O46" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P46" s="74"/>
+      <c r="P46" s="152"/>
       <c r="Q46" s="34"/>
     </row>
-    <row r="47" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" s="29" customFormat="1">
       <c r="A47" s="27">
         <v>35</v>
       </c>
@@ -4677,10 +4678,10 @@
       <c r="O47" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P47" s="74"/>
+      <c r="P47" s="152"/>
       <c r="Q47" s="34"/>
     </row>
-    <row r="48" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" s="29" customFormat="1">
       <c r="A48" s="27"/>
       <c r="B48" s="27"/>
       <c r="C48" s="30"/>
@@ -4696,10 +4697,10 @@
       <c r="M48" s="46"/>
       <c r="N48" s="46"/>
       <c r="O48" s="46"/>
-      <c r="P48" s="74"/>
+      <c r="P48" s="152"/>
       <c r="Q48" s="34"/>
     </row>
-    <row r="49" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="29" customFormat="1">
       <c r="A49" s="27">
         <v>36</v>
       </c>
@@ -4737,10 +4738,10 @@
       <c r="O49" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P49" s="72"/>
+      <c r="P49" s="150"/>
       <c r="Q49" s="34"/>
     </row>
-    <row r="50" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="29" customFormat="1">
       <c r="A50" s="27"/>
       <c r="B50" s="27"/>
       <c r="C50" s="30"/>
@@ -4759,7 +4760,7 @@
       <c r="P50" s="27"/>
       <c r="Q50" s="34"/>
     </row>
-    <row r="51" spans="1:17" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="29" customFormat="1" ht="12.75" customHeight="1">
       <c r="A51" s="27">
         <v>37</v>
       </c>
@@ -4797,12 +4798,12 @@
       <c r="O51" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P51" s="71" t="s">
+      <c r="P51" s="149" t="s">
         <v>36</v>
       </c>
       <c r="Q51" s="34"/>
     </row>
-    <row r="52" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="29" customFormat="1">
       <c r="A52" s="27">
         <v>38</v>
       </c>
@@ -4840,10 +4841,10 @@
       <c r="O52" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P52" s="74"/>
+      <c r="P52" s="152"/>
       <c r="Q52" s="34"/>
     </row>
-    <row r="53" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="29" customFormat="1">
       <c r="A53" s="27">
         <v>39</v>
       </c>
@@ -4881,10 +4882,10 @@
       <c r="O53" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P53" s="74"/>
+      <c r="P53" s="152"/>
       <c r="Q53" s="34"/>
     </row>
-    <row r="54" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" s="29" customFormat="1">
       <c r="A54" s="27">
         <v>40</v>
       </c>
@@ -4922,10 +4923,10 @@
       <c r="O54" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P54" s="74"/>
+      <c r="P54" s="152"/>
       <c r="Q54" s="34"/>
     </row>
-    <row r="55" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" s="29" customFormat="1">
       <c r="A55" s="27">
         <v>41</v>
       </c>
@@ -4963,10 +4964,10 @@
       <c r="O55" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P55" s="72"/>
+      <c r="P55" s="150"/>
       <c r="Q55" s="34"/>
     </row>
-    <row r="56" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" s="29" customFormat="1">
       <c r="A56" s="27">
         <v>42</v>
       </c>
@@ -5004,14 +5005,14 @@
       <c r="O56" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P56" s="71" t="s">
+      <c r="P56" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="Q56" s="73" t="s">
+      <c r="Q56" s="151" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" s="29" customFormat="1">
       <c r="A57" s="27">
         <v>43</v>
       </c>
@@ -5049,10 +5050,10 @@
       <c r="O57" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P57" s="72"/>
-      <c r="Q57" s="73"/>
-    </row>
-    <row r="58" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P57" s="150"/>
+      <c r="Q57" s="151"/>
+    </row>
+    <row r="58" spans="1:17" s="29" customFormat="1">
       <c r="A58" s="27"/>
       <c r="B58" s="27"/>
       <c r="C58" s="30"/>
@@ -5071,7 +5072,7 @@
       <c r="P58" s="27"/>
       <c r="Q58" s="27"/>
     </row>
-    <row r="59" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" s="29" customFormat="1">
       <c r="A59" s="27">
         <v>45</v>
       </c>
@@ -5114,7 +5115,7 @@
       </c>
       <c r="Q59" s="34"/>
     </row>
-    <row r="60" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" s="29" customFormat="1">
       <c r="A60" s="27">
         <v>46</v>
       </c>
@@ -5157,7 +5158,7 @@
       </c>
       <c r="Q60" s="34"/>
     </row>
-    <row r="61" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" s="29" customFormat="1">
       <c r="A61" s="27">
         <v>47</v>
       </c>
@@ -5200,7 +5201,7 @@
       </c>
       <c r="Q61" s="34"/>
     </row>
-    <row r="62" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" s="29" customFormat="1">
       <c r="A62" s="27">
         <v>48</v>
       </c>
@@ -5243,7 +5244,7 @@
       </c>
       <c r="Q62" s="34"/>
     </row>
-    <row r="63" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" s="29" customFormat="1">
       <c r="A63" s="27">
         <v>49</v>
       </c>
@@ -5286,7 +5287,7 @@
       </c>
       <c r="Q63" s="34"/>
     </row>
-    <row r="64" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" s="29" customFormat="1">
       <c r="A64" s="27">
         <v>50</v>
       </c>
@@ -5329,7 +5330,7 @@
       </c>
       <c r="Q64" s="34"/>
     </row>
-    <row r="65" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" s="29" customFormat="1">
       <c r="A65" s="27">
         <v>51</v>
       </c>
@@ -5372,7 +5373,7 @@
       </c>
       <c r="Q65" s="34"/>
     </row>
-    <row r="66" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" s="29" customFormat="1">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="49"/>
@@ -5391,7 +5392,7 @@
       <c r="P66" s="39"/>
       <c r="Q66" s="34"/>
     </row>
-    <row r="67" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" s="29" customFormat="1">
       <c r="A67" s="16"/>
       <c r="B67" s="16"/>
       <c r="C67" s="48" t="s">
@@ -5412,7 +5413,7 @@
       <c r="P67" s="27"/>
       <c r="Q67" s="34"/>
     </row>
-    <row r="68" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" s="29" customFormat="1">
       <c r="A68" s="27">
         <v>52</v>
       </c>
@@ -5450,12 +5451,12 @@
       <c r="O68" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P68" s="71" t="s">
+      <c r="P68" s="149" t="s">
         <v>117</v>
       </c>
       <c r="Q68" s="34"/>
     </row>
-    <row r="69" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" s="29" customFormat="1">
       <c r="A69" s="27">
         <v>53</v>
       </c>
@@ -5493,10 +5494,10 @@
       <c r="O69" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P69" s="74"/>
+      <c r="P69" s="152"/>
       <c r="Q69" s="34"/>
     </row>
-    <row r="70" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" s="29" customFormat="1">
       <c r="A70" s="27">
         <v>54</v>
       </c>
@@ -5534,10 +5535,10 @@
       <c r="O70" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P70" s="74"/>
+      <c r="P70" s="152"/>
       <c r="Q70" s="34"/>
     </row>
-    <row r="71" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" s="29" customFormat="1">
       <c r="A71" s="27">
         <v>55</v>
       </c>
@@ -5575,10 +5576,10 @@
       <c r="O71" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P71" s="74"/>
+      <c r="P71" s="152"/>
       <c r="Q71" s="34"/>
     </row>
-    <row r="72" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" s="29" customFormat="1">
       <c r="A72" s="27">
         <v>56</v>
       </c>
@@ -5616,10 +5617,10 @@
       <c r="O72" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P72" s="74"/>
+      <c r="P72" s="152"/>
       <c r="Q72" s="34"/>
     </row>
-    <row r="73" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" s="29" customFormat="1">
       <c r="A73" s="27">
         <v>57</v>
       </c>
@@ -5657,10 +5658,10 @@
       <c r="O73" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P73" s="74"/>
+      <c r="P73" s="152"/>
       <c r="Q73" s="34"/>
     </row>
-    <row r="74" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" s="29" customFormat="1">
       <c r="A74" s="27">
         <v>58</v>
       </c>
@@ -5698,10 +5699,10 @@
       <c r="O74" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="P74" s="74"/>
+      <c r="P74" s="152"/>
       <c r="Q74" s="34"/>
     </row>
-    <row r="75" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" s="29" customFormat="1">
       <c r="A75" s="27"/>
       <c r="B75" s="27"/>
       <c r="C75" s="30"/>
@@ -5717,10 +5718,10 @@
       <c r="M75" s="46"/>
       <c r="N75" s="46"/>
       <c r="O75" s="46"/>
-      <c r="P75" s="74"/>
+      <c r="P75" s="152"/>
       <c r="Q75" s="34"/>
     </row>
-    <row r="76" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" s="29" customFormat="1">
       <c r="A76" s="27">
         <v>59</v>
       </c>
@@ -5758,10 +5759,10 @@
       <c r="O76" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P76" s="74"/>
+      <c r="P76" s="152"/>
       <c r="Q76" s="34"/>
     </row>
-    <row r="77" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" s="29" customFormat="1">
       <c r="A77" s="27">
         <v>60</v>
       </c>
@@ -5799,10 +5800,10 @@
       <c r="O77" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P77" s="74"/>
+      <c r="P77" s="152"/>
       <c r="Q77" s="34"/>
     </row>
-    <row r="78" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" s="29" customFormat="1">
       <c r="A78" s="27">
         <v>61</v>
       </c>
@@ -5840,10 +5841,10 @@
       <c r="O78" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="P78" s="72"/>
+      <c r="P78" s="150"/>
       <c r="Q78" s="34"/>
     </row>
-    <row r="79" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" s="29" customFormat="1">
       <c r="A79" s="27"/>
       <c r="B79" s="27"/>
       <c r="C79" s="30"/>
@@ -5862,7 +5863,7 @@
       <c r="P79" s="27"/>
       <c r="Q79" s="34"/>
     </row>
-    <row r="80" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" s="29" customFormat="1">
       <c r="A80" s="27">
         <v>62</v>
       </c>
@@ -5905,7 +5906,7 @@
       </c>
       <c r="Q80" s="34"/>
     </row>
-    <row r="81" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="29" customFormat="1">
       <c r="A81" s="27">
         <v>63</v>
       </c>
@@ -5948,7 +5949,7 @@
       </c>
       <c r="Q81" s="34"/>
     </row>
-    <row r="82" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="29" customFormat="1">
       <c r="A82" s="27">
         <v>64</v>
       </c>
@@ -5991,7 +5992,7 @@
       </c>
       <c r="Q82" s="34"/>
     </row>
-    <row r="83" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" s="29" customFormat="1">
       <c r="A83" s="27">
         <v>65</v>
       </c>
@@ -6034,7 +6035,7 @@
       </c>
       <c r="Q83" s="34"/>
     </row>
-    <row r="84" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" s="29" customFormat="1">
       <c r="A84" s="27">
         <v>66</v>
       </c>
@@ -6077,7 +6078,7 @@
       </c>
       <c r="Q84" s="34"/>
     </row>
-    <row r="85" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" s="29" customFormat="1">
       <c r="A85" s="27">
         <v>67</v>
       </c>
@@ -6120,7 +6121,7 @@
       </c>
       <c r="Q85" s="34"/>
     </row>
-    <row r="86" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" s="29" customFormat="1">
       <c r="A86" s="27"/>
       <c r="B86" s="27"/>
       <c r="C86" s="30"/>
@@ -6139,7 +6140,7 @@
       <c r="P86" s="27"/>
       <c r="Q86" s="34"/>
     </row>
-    <row r="87" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" s="29" customFormat="1">
       <c r="A87" s="27">
         <v>68</v>
       </c>
@@ -6182,7 +6183,7 @@
       </c>
       <c r="Q87" s="34"/>
     </row>
-    <row r="88" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" s="29" customFormat="1">
       <c r="A88" s="27">
         <v>69</v>
       </c>
@@ -6225,7 +6226,7 @@
       </c>
       <c r="Q88" s="34"/>
     </row>
-    <row r="89" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" s="29" customFormat="1">
       <c r="A89" s="27">
         <v>70</v>
       </c>
@@ -6268,7 +6269,7 @@
       </c>
       <c r="Q89" s="34"/>
     </row>
-    <row r="90" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" s="29" customFormat="1">
       <c r="A90" s="27">
         <v>71</v>
       </c>
@@ -6311,7 +6312,7 @@
       </c>
       <c r="Q90" s="34"/>
     </row>
-    <row r="91" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" s="29" customFormat="1">
       <c r="A91" s="27">
         <v>72</v>
       </c>
@@ -6354,7 +6355,7 @@
       </c>
       <c r="Q91" s="34"/>
     </row>
-    <row r="92" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" s="29" customFormat="1">
       <c r="A92" s="27">
         <v>73</v>
       </c>
@@ -6397,7 +6398,7 @@
       </c>
       <c r="Q92" s="34"/>
     </row>
-    <row r="93" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" s="29" customFormat="1">
       <c r="A93" s="27">
         <v>74</v>
       </c>
@@ -6440,7 +6441,7 @@
       </c>
       <c r="Q93" s="34"/>
     </row>
-    <row r="94" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" s="29" customFormat="1">
       <c r="A94" s="27"/>
       <c r="B94" s="27"/>
       <c r="C94" s="30"/>
@@ -6459,7 +6460,7 @@
       <c r="P94" s="27"/>
       <c r="Q94" s="34"/>
     </row>
-    <row r="95" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" s="15" customFormat="1">
       <c r="A95" s="42"/>
       <c r="B95" s="42"/>
       <c r="C95" s="48" t="s">
@@ -6480,7 +6481,7 @@
       <c r="P95" s="33"/>
       <c r="Q95" s="33"/>
     </row>
-    <row r="96" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" s="15" customFormat="1">
       <c r="A96" s="16">
         <v>75</v>
       </c>
@@ -6525,7 +6526,7 @@
       </c>
       <c r="Q96" s="34"/>
     </row>
-    <row r="97" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" s="15" customFormat="1">
       <c r="A97" s="16">
         <v>76</v>
       </c>
@@ -6570,7 +6571,7 @@
       </c>
       <c r="Q97" s="34"/>
     </row>
-    <row r="98" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" s="15" customFormat="1">
       <c r="A98" s="16">
         <v>77</v>
       </c>
@@ -6615,7 +6616,7 @@
       </c>
       <c r="Q98" s="34"/>
     </row>
-    <row r="99" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" s="15" customFormat="1">
       <c r="A99" s="16">
         <v>78</v>
       </c>
@@ -6660,7 +6661,7 @@
       </c>
       <c r="Q99" s="34"/>
     </row>
-    <row r="100" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" s="15" customFormat="1">
       <c r="A100" s="16">
         <v>79</v>
       </c>
@@ -6705,7 +6706,7 @@
       </c>
       <c r="Q100" s="34"/>
     </row>
-    <row r="101" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" s="15" customFormat="1">
       <c r="A101" s="16">
         <v>80</v>
       </c>
@@ -6750,7 +6751,7 @@
       </c>
       <c r="Q101" s="34"/>
     </row>
-    <row r="102" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" s="15" customFormat="1">
       <c r="A102" s="16">
         <v>81</v>
       </c>
@@ -6795,7 +6796,7 @@
       </c>
       <c r="Q102" s="34"/>
     </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" s="15" customFormat="1">
       <c r="A103" s="16">
         <v>82</v>
       </c>
@@ -6840,7 +6841,7 @@
       </c>
       <c r="Q103" s="34"/>
     </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" s="15" customFormat="1">
       <c r="A104" s="16">
         <v>83</v>
       </c>
@@ -6885,7 +6886,7 @@
       </c>
       <c r="Q104" s="34"/>
     </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" s="15" customFormat="1">
       <c r="A105" s="16">
         <v>84</v>
       </c>
@@ -6930,7 +6931,7 @@
       </c>
       <c r="Q105" s="34"/>
     </row>
-    <row r="106" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" s="15" customFormat="1">
       <c r="A106" s="16">
         <v>85</v>
       </c>
@@ -6975,7 +6976,7 @@
       </c>
       <c r="Q106" s="34"/>
     </row>
-    <row r="107" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" s="15" customFormat="1">
       <c r="A107" s="16">
         <v>86</v>
       </c>
@@ -7020,7 +7021,7 @@
       </c>
       <c r="Q107" s="34"/>
     </row>
-    <row r="108" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" s="15" customFormat="1">
       <c r="A108" s="16">
         <v>87</v>
       </c>
@@ -7065,7 +7066,7 @@
       </c>
       <c r="Q108" s="34"/>
     </row>
-    <row r="109" spans="1:17" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" s="15" customFormat="1" ht="16.5" customHeight="1">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="23"/>
@@ -7084,19 +7085,19 @@
       <c r="P109" s="35"/>
       <c r="Q109" s="17"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17">
       <c r="D110" s="10"/>
       <c r="E110" s="10"/>
       <c r="F110" s="10"/>
       <c r="J110" s="10"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17">
       <c r="D111" s="10"/>
       <c r="E111" s="10"/>
       <c r="F111" s="10"/>
       <c r="J111" s="10"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -7105,18 +7106,18 @@
       <c r="F112" s="11"/>
       <c r="J112" s="11"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" t="s">
         <v>113</v>
       </c>

</xml_diff>